<commit_message>
Add test case 2
</commit_message>
<xml_diff>
--- a/Guru99_Live_Project_Demo_TestCase.xlsx
+++ b/Guru99_Live_Project_Demo_TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray.guo/Documents/workshop/test/Guru99_Ecommerce_Java_Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A287DFB-6700-4A46-A8F0-D490D16E6322}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D600440E-082D-9142-827F-3F0A0C017A4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1000" windowWidth="28160" windowHeight="15080" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
+    <workbookView xWindow="2980" yWindow="5120" windowWidth="28160" windowHeight="15080" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Case ID</t>
   </si>
@@ -62,6 +62,20 @@
     <t>1. Text 'This is demo site' shown in home page
 2. Title 'Mobile' is shown on mobile list page.
 3. All 3 prodcuts sorted by name</t>
+  </si>
+  <si>
+    <t>Verify that cost of product in list page and details page are equal</t>
+  </si>
+  <si>
+    <t>1. Goto http://live.demoguru99.com
+2. Cick one mobile menu
+3. In the list of all mobile, read the cost of sony xperia mobile. note this value
+4. Click on Sony Xperia mobile
+5. Read the Sony xoperia mobile from detail page
+6. Compare value in step 3 &amp; 5</t>
+  </si>
+  <si>
+    <t>Product value in list and details page should be equal($100)</t>
   </si>
 </sst>
 </file>
@@ -131,9 +145,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -141,10 +152,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,50 +474,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AED6A07-176F-FF4B-8B05-2F1BF9F8079C}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35.5" customWidth="1"/>
-    <col min="3" max="3" width="69.83203125" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="49.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="69.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add test case 3
</commit_message>
<xml_diff>
--- a/Guru99_Live_Project_Demo_TestCase.xlsx
+++ b/Guru99_Live_Project_Demo_TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray.guo/Documents/workshop/test/Guru99_Ecommerce_Java_Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D600440E-082D-9142-827F-3F0A0C017A4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7577D70A-B20E-2C45-8C39-96CFDE629789}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="5120" windowWidth="28160" windowHeight="15080" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
+    <workbookView xWindow="920" yWindow="6120" windowWidth="27240" windowHeight="12420" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Case ID</t>
   </si>
@@ -76,6 +76,22 @@
   </si>
   <si>
     <t>Product value in list and details page should be equal($100)</t>
+  </si>
+  <si>
+    <t>Verify that you can not add more product in cart that the product avaliabke in store</t>
+  </si>
+  <si>
+    <t>1. Goto http://live.demoguru99.com
+2. Cick one mobile menu
+3. In the list of all mobile, click on "add to cart" for sony xperia mobile. 
+4. Change "QTY" value to1000 and click "update" button
+5. verify the error message
+6. Then cilck on "Empty cart" link in the footer of list of all mobiules
+7. Verify cart is empty</t>
+  </si>
+  <si>
+    <t>1. On clicking update button an error is shown 'The requested quantity for "Sony Xperia" is not avaliable.'
+2. On clicking empty cart button - a message 'Shopping cart is empty' is shown</t>
   </si>
 </sst>
 </file>
@@ -476,7 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AED6A07-176F-FF4B-8B05-2F1BF9F8079C}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -535,12 +551,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+    <row r="4" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>

</xml_diff>

<commit_message>
Add test case 4 steps into excel
</commit_message>
<xml_diff>
--- a/Guru99_Live_Project_Demo_TestCase.xlsx
+++ b/Guru99_Live_Project_Demo_TestCase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray.guo/Documents/workshop/test/Guru99_Ecommerce_Java_Demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray.guo/Documents/workshop/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7577D70A-B20E-2C45-8C39-96CFDE629789}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B794A938-BF54-2544-B6A2-4C5FB9667748}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="6120" windowWidth="27240" windowHeight="12420" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Case ID</t>
   </si>
@@ -92,6 +92,25 @@
   <si>
     <t>1. On clicking update button an error is shown 'The requested quantity for "Sony Xperia" is not avaliable.'
 2. On clicking empty cart button - a message 'Shopping cart is empty' is shown</t>
+  </si>
+  <si>
+    <t>Verify that you are abke to compare two products</t>
+  </si>
+  <si>
+    <t>1. Goto http://live.demoguru99.com
+2. Cick one mobile menu
+3. In mobile products list, click on "add to compare" for 2 mobile
+4. Click on 'Compare'
+5. verify the pop-up window and check that the products are reflected in it
+6. Close the popup windows</t>
+  </si>
+  <si>
+    <t>Phone 1 - Sony Xperia
+Phone 2 - Iphone</t>
+  </si>
+  <si>
+    <t>1. A popup window opens with heading as 'Compare products' and the selected products are present in it.
+2. Popup window is closed</t>
   </si>
 </sst>
 </file>
@@ -492,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AED6A07-176F-FF4B-8B05-2F1BF9F8079C}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,12 +585,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+    <row r="5" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>

</xml_diff>

<commit_message>
Add test case 5
</commit_message>
<xml_diff>
--- a/Guru99_Live_Project_Demo_TestCase.xlsx
+++ b/Guru99_Live_Project_Demo_TestCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray.guo/Documents/workshop/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B794A938-BF54-2544-B6A2-4C5FB9667748}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA2A4FA-D316-8D46-9C5C-71B8EC52DEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="6120" windowWidth="27240" windowHeight="12420" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
+    <workbookView xWindow="1300" yWindow="7320" windowWidth="27240" windowHeight="12420" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Case ID</t>
   </si>
@@ -111,6 +111,28 @@
   <si>
     <t>1. A popup window opens with heading as 'Compare products' and the selected products are present in it.
 2. Popup window is closed</t>
+  </si>
+  <si>
+    <t>Verify you can create account in E-commerce site and can share wishlist to other people using email</t>
+  </si>
+  <si>
+    <t>1. Goto http://live.demoguru99.com
+2. Click on my account link
+3. Click Create account link and fill new user information exoect email id
+4. Click register
+5. verify registration is done
+6. goto Tv menu
+7. Add product in your wish list
+8. Click share wishlist
+9. In next page enter Email and a message and click share wishlist
+10. Check wishlist is shared</t>
+  </si>
+  <si>
+    <t>product = LOG LCD</t>
+  </si>
+  <si>
+    <t>1. Account registration done
+2. Wishlist Shared Successfully</t>
   </si>
 </sst>
 </file>
@@ -511,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AED6A07-176F-FF4B-8B05-2F1BF9F8079C}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,12 +624,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+    <row r="6" spans="1:5" ht="200" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
add tset case 6
</commit_message>
<xml_diff>
--- a/Guru99_Live_Project_Demo_TestCase.xlsx
+++ b/Guru99_Live_Project_Demo_TestCase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray.guo/Documents/workshop/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray.guo/Documents/workshop/person/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA2A4FA-D316-8D46-9C5C-71B8EC52DEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A063E1-32F4-AB48-910B-FDC5B7878D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="7320" windowWidth="27240" windowHeight="12420" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
+    <workbookView xWindow="1060" yWindow="5300" windowWidth="27240" windowHeight="12420" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Case ID</t>
   </si>
@@ -116,23 +116,79 @@
     <t>Verify you can create account in E-commerce site and can share wishlist to other people using email</t>
   </si>
   <si>
+    <t>product = LOG LCD</t>
+  </si>
+  <si>
+    <t>1. Account registration done
+2. Wishlist Shared Successfully</t>
+  </si>
+  <si>
+    <t>Verify user is able to purchase product using registed email id(Use chrome browser)</t>
+  </si>
+  <si>
     <t>1. Goto http://live.demoguru99.com
 2. Click on my account link
-3. Click Create account link and fill new user information exoect email id
-4. Click register
-5. verify registration is done
-6. goto Tv menu
-7. Add product in your wish list
-8. Click share wishlist
-9. In next page enter Email and a message and click share wishlist
-10. Check wishlist is shared</t>
-  </si>
-  <si>
-    <t>product = LOG LCD</t>
-  </si>
-  <si>
-    <t>1. Account registration done
-2. Wishlist Shared Successfully</t>
+4. login
+5. goto Tv menu
+6. Add product in your wish list
+7. Click share wishlist
+8. In next page enter Email and a message and click share wishlist
+9. Check wishlist is shared</t>
+  </si>
+  <si>
+    <t>1. Goto http://live.demoguru99.com
+2. Click on my account link
+3. Loing in application
+4. Click on my wishlist link
+5. In next oage, click add to cart link
+6. Click proceed to checkout 
+7.enter shipping information
+8. click estimate
+9. verify shipping cost generated
+10. select shipping cost.update total
+11. verify shipping cost is add t total
+12. click 'Proceed to checkout"
+13. Enter billing information
+14. In shipping method, click continue
+15. In payment informtaion select 'Check/Money order' radio button. Click continue
+16. Click 'Place order' button
+17. Verify order is generated. Note the order number</t>
+  </si>
+  <si>
+    <t>1. Shipping information country = united states 
+state =  new york
+zip = 542896
+address = ABC 
+city = new york
+Telephone = 12345678</t>
+  </si>
+  <si>
+    <t>1. flat rate shipping of $5 is generated
+2.Shipping cost is added to total product cost
+3.Order is placed. Order number is generated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that you will be able ot save previously placed order as a pdf file </t>
+  </si>
+  <si>
+    <t>1. Go to http://live. Demoguru99.com
+2. Click on my account link 
+3. Login in application
+4. Click on 'My Orders'
+5. Click on 'View order'
+6. Verify the previously created order is displayed in 'recent orders' table and status is pending
+7. Click on 'print order' link
+8. Verify order is saved as PDF</t>
+  </si>
+  <si>
+    <t>Use FireFox</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1. Previously created order is displayed in 'Recent orders' table and status is pending 
+2. Order is saved as PDF</t>
   </si>
 </sst>
 </file>
@@ -197,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -216,6 +272,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AED6A07-176F-FF4B-8B05-2F1BF9F8079C}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,7 +606,7 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -562,7 +621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -577,7 +636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="140" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -592,7 +651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="140" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -607,7 +666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="140" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="140" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -624,7 +683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="200" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -632,72 +691,97 @@
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="351" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="180" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="E9" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>

</xml_diff>

<commit_message>
finish the test case 6 and add it into the test suit file
</commit_message>
<xml_diff>
--- a/Guru99_Live_Project_Demo_TestCase.xlsx
+++ b/Guru99_Live_Project_Demo_TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray.guo/Documents/workshop/person/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A063E1-32F4-AB48-910B-FDC5B7878D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDF67FB-B112-D64C-B6A8-AA9BD5A9ECB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="5300" windowWidth="27240" windowHeight="12420" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
+    <workbookView xWindow="3360" yWindow="940" windowWidth="27240" windowHeight="16120" xr2:uid="{F81677D8-A7CC-654E-814A-EA03B107371E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AED6A07-176F-FF4B-8B05-2F1BF9F8079C}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>